<commit_message>
Atualização Backlog - Para a SP3
</commit_message>
<xml_diff>
--- a/Documentação/GraficoBurndown_aggran_grupo09.xlsx
+++ b/Documentação/GraficoBurndown_aggran_grupo09.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesley.souza\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{74048B46-8C72-4748-B6A3-AC1E8536FEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D8D85C5-E592-48C0-B8DD-833EFAC4FA0F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC4E9840-4199-44F7-BC07-94FB6D44FCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A7B2C129-0DC2-486F-98D2-A2B5534F11BE}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="98">
   <si>
     <t>Aggran</t>
   </si>
@@ -224,18 +224,6 @@
     <t>Realizar a instalação do MySQL no ambiente de virtualização</t>
   </si>
   <si>
-    <t>API de endereço</t>
-  </si>
-  <si>
-    <t>Interligar o CEP do cadastro a API de Endereço (ViaCEP)</t>
-  </si>
-  <si>
-    <t>API de registro</t>
-  </si>
-  <si>
-    <t>Interligar ao banco de dados a API que irá inserir os dados informados pelos clientes no registro</t>
-  </si>
-  <si>
     <t>Tela de login</t>
   </si>
   <si>
@@ -254,60 +242,9 @@
     <t>Teste com Sensor do Projeto + Gráficos</t>
   </si>
   <si>
-    <t>Atualização do sistema</t>
-  </si>
-  <si>
-    <t>Deverá atualizar o sistema a cada 10 minutos</t>
-  </si>
-  <si>
-    <t>Desempenho</t>
-  </si>
-  <si>
-    <t>Deverá conseguir suportar requisições de mais de um cliente</t>
-  </si>
-  <si>
-    <t>Segurança</t>
-  </si>
-  <si>
-    <t>Deverá conter sistema de criptografia para proteção dos dados em conformidade com o LGPD</t>
-  </si>
-  <si>
-    <t>Usabilidade</t>
-  </si>
-  <si>
-    <t>Deverá ser de fácil usuabilidade</t>
-  </si>
-  <si>
-    <t>Confiabilidade</t>
-  </si>
-  <si>
-    <t>Deverá ter capacidade de manter o sistema funcionando</t>
-  </si>
-  <si>
-    <t>Escalabilidade</t>
-  </si>
-  <si>
-    <t>Deverá suportar aumento de clientes utilizando o sistema</t>
-  </si>
-  <si>
-    <t>Compatibilidade</t>
-  </si>
-  <si>
-    <t>Deverá ser compatível a navegadores como chrome e edge</t>
-  </si>
-  <si>
-    <t>API integrado ao site</t>
-  </si>
-  <si>
     <t>Será integrado a API que realizará selects que serão utilizados para a criação dos gráficos e mostrados no site</t>
   </si>
   <si>
-    <t>Página sobre a empresa</t>
-  </si>
-  <si>
-    <t>Conterá as informações inerentes a empresa e seus objetivos</t>
-  </si>
-  <si>
     <t>Página Fale conosco</t>
   </si>
   <si>
@@ -330,13 +267,94 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>API integrado ao site - WEB-DATA-VIZ</t>
+  </si>
+  <si>
+    <t>Manual de instalação</t>
+  </si>
+  <si>
+    <t>Conterá o manual de como a nossa solução IoT deverá ser instalada após recebe-la</t>
+  </si>
+  <si>
+    <t>Documentação final do projeto</t>
+  </si>
+  <si>
+    <t>No qual, estará comtodas as informações referentes ao projeto em sua última Sprint</t>
+  </si>
+  <si>
+    <t>PPT de apresentação do grupo</t>
+  </si>
+  <si>
+    <t>Será a versão final da nossa apresentação, que conterá todos os detalhes do projeto</t>
+  </si>
+  <si>
+    <t>Site institucional - versão final</t>
+  </si>
+  <si>
+    <t>Conterá neste momento todas as páginas e será conectado a nossa API</t>
+  </si>
+  <si>
+    <t>Cadastro, login e dashboard, conectado ao BD</t>
+  </si>
+  <si>
+    <t>As páginas citadas estarão conectadas ao banco de dados, com a implementação da API web-data-viz</t>
+  </si>
+  <si>
+    <t>Fluxograma do processo de atendimento do suporte</t>
+  </si>
+  <si>
+    <t>Conterá o paaso a passo a ser seguido para o suporte quando ocorrer algum incidente, problema ou requisição do nosso cliente</t>
+  </si>
+  <si>
+    <t>Ferramenta do processo de atendimento do suporte - Jira</t>
+  </si>
+  <si>
+    <t>Será o nosso help desk, no qual, é o meio de comunicação do nosso cliente e o nosso suporte</t>
+  </si>
+  <si>
+    <t>GMUD - Documento de gestão de Mudanças</t>
+  </si>
+  <si>
+    <t>Conterá os passos que deverão ser seguidos quando precisar realizar alguma mudança de TI, sendo eles, Emergencial, normal e padrão</t>
+  </si>
+  <si>
+    <t>Modelagem lógica - final</t>
+  </si>
+  <si>
+    <t>Conterá nossas tabelas referentes ao nosso modelo de negócio, para uma melhor vizualização do nosso BD</t>
+  </si>
+  <si>
+    <t>Tabelas criadas</t>
+  </si>
+  <si>
+    <t>Tabelas referentes ao nosso modelo de negócio já funcionando e com os inserts necessários para a realização de insight</t>
+  </si>
+  <si>
+    <t>Views para dashboard</t>
+  </si>
+  <si>
+    <t>No qual, será os selects necessário para a realização da vizualização no dashboard</t>
+  </si>
+  <si>
+    <t>Solução IoT - conectada e funcionado</t>
+  </si>
+  <si>
+    <t>É a parte do hardware do nosso projeto, será necessária para a coleta de dados</t>
+  </si>
+  <si>
+    <t>Distribuição em duas máquinas</t>
+  </si>
+  <si>
+    <t>No qual, o nosso projeto será separado em duas máquinas, uma que conterá a coleta de dados e arduino e a outra será para o BD e a aplicação na VM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +380,19 @@
       <sz val="48"/>
       <color rgb="FF339933"/>
       <name val="Anton"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -420,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -520,11 +551,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -596,6 +642,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -954,9 +1009,9 @@
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[VALOR]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="pt-BR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -991,9 +1046,9 @@
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[VALOR]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="pt-BR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1162,9 +1217,9 @@
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[VALOR]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="pt-BR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1199,9 +1254,9 @@
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[VALOR]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="pt-BR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1236,9 +1291,9 @@
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[VALOR]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="pt-BR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1341,10 +1396,10 @@
                   <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2067,15 +2122,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>859154</xdr:colOff>
+      <xdr:colOff>2391620</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>48683</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4490085</xdr:colOff>
+      <xdr:colOff>6022551</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:rowOff>286808</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2099,7 +2154,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3535679" y="57150"/>
+          <a:off x="5795220" y="48683"/>
           <a:ext cx="3630931" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2119,7 +2174,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2163,10 +2218,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9FEA6928-F3E9-41BC-B8A2-9403BBB8FB3D}" name="Tabela2" displayName="Tabela2" ref="A2:H33" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17">
-  <autoFilter ref="A2" xr:uid="{9FEA6928-F3E9-41BC-B8A2-9403BBB8FB3D}">
-    <filterColumn colId="0" hiddenButton="1"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9FEA6928-F3E9-41BC-B8A2-9403BBB8FB3D}" name="Tabela2" displayName="Tabela2" ref="A2:H36" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0DE55F2E-7BDE-405D-AB99-082B00C7800E}" name="REQUISITOS"/>
     <tableColumn id="2" xr3:uid="{FFD63478-5104-45C9-9386-12AB16A25B6F}" name="DESCRIÇÃO"/>
@@ -2524,30 +2576,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C44B03-923B-4AFE-8D99-0AB4AE36770F}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="127.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="87.6" customHeight="1">
@@ -2632,8 +2684,8 @@
         <v>19</v>
       </c>
       <c r="K3" s="12">
-        <f>SUM($E$3:$E$33)</f>
-        <v>302</v>
+        <f>SUM($E$3:$E$36)</f>
+        <v>299</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -2668,7 +2720,7 @@
         <v>18</v>
       </c>
       <c r="K4" s="12">
-        <f>SUMIF($G$3:$G$33,J4,$E$3:$E$33)</f>
+        <f>SUMIF($G$3:$G$36,J4,$E$3:$E$36)</f>
         <v>79</v>
       </c>
       <c r="L4" s="2">
@@ -2712,7 +2764,7 @@
         <v>26</v>
       </c>
       <c r="K5" s="12">
-        <f>SUMIF($G$3:$G$33,J5,$E$3:$E$33)</f>
+        <f>SUMIF($G$3:$G$36,J5,$E$3:$E$36)</f>
         <v>79</v>
       </c>
       <c r="L5" s="2">
@@ -2721,11 +2773,11 @@
       </c>
       <c r="M5" s="2">
         <f>SUMIFS(Tabela2[TAM('#)],Tabela2[STATUS],$M$2,Tabela2[SPRINT],$J5)</f>
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="N5" s="2">
         <f>L5-M5</f>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2757,20 +2809,20 @@
         <v>30</v>
       </c>
       <c r="K6" s="12">
-        <f>SUMIF($G$3:$G$33,J6,$E$3:$E$33)</f>
-        <v>144</v>
+        <f>SUMIF($G$3:$G$36,J6,$E$3:$E$36)</f>
+        <v>141</v>
       </c>
       <c r="L6" s="2">
         <f>SUMIF(Tabela2[SPRINT],J6,Tabela2[TAM('#)])</f>
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M6" s="2">
         <f>SUMIFS(Tabela2[TAM('#)],Tabela2[STATUS],$M$2,Tabela2[SPRINT],$J6)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="N6" s="2">
         <f>L6-M6</f>
-        <v>144</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2802,8 +2854,8 @@
         <v>33</v>
       </c>
       <c r="K7" s="24">
-        <f>ROUND(AVERAGE($E$3:$E$33),2)</f>
-        <v>9.74</v>
+        <f>ROUND(AVERAGE($E$3:$E$36),2)</f>
+        <v>8.7899999999999991</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -3016,7 +3068,7 @@
         <v>26</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -3042,7 +3094,7 @@
         <v>26</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3082,19 +3134,19 @@
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E18" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3117,10 +3169,10 @@
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3131,16 +3183,16 @@
         <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E20" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>26</v>
@@ -3151,10 +3203,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
@@ -3169,21 +3221,21 @@
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -3192,30 +3244,30 @@
         <v>5</v>
       </c>
       <c r="F22" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E23" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -3229,13 +3281,13 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>39</v>
@@ -3244,7 +3296,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>30</v>
@@ -3255,13 +3307,13 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>39</v>
@@ -3270,7 +3322,7 @@
         <v>13</v>
       </c>
       <c r="F25" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>30</v>
@@ -3281,39 +3333,39 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E26" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>39</v>
@@ -3322,7 +3374,7 @@
         <v>13</v>
       </c>
       <c r="F27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>30</v>
@@ -3333,22 +3385,22 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E28" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>30</v>
@@ -3359,65 +3411,65 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E30" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F30" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>16</v>
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -3436,46 +3488,46 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>29</v>
+      <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E32" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="1">
         <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="1">
-        <v>8</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -3484,6 +3536,84 @@
         <v>30</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="1">
+        <v>13</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1">
+        <v>8</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3497,24 +3627,30 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C524FE3C-4B8B-40A4-B475-13B25C2453B6}">
           <x14:formula1>
             <xm:f>'Lista - validações'!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D33</xm:sqref>
+          <xm:sqref>D3:D36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0521648B-37EF-44B0-BC8C-15BDEE9F5389}">
           <x14:formula1>
             <xm:f>'Lista - validações'!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E33</xm:sqref>
+          <xm:sqref>E3:E36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4CD2968B-4110-4B19-8048-4CBD7F3EEB11}">
           <x14:formula1>
             <xm:f>'Lista - validações'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H33</xm:sqref>
+          <xm:sqref>H3:H36</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4356CA9A-8686-440C-917A-689F0E50EDF0}">
+          <x14:formula1>
+            <xm:f>'Lista - validações'!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3527,18 +3663,18 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="18"/>
-    <col min="6" max="7" width="12.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="18"/>
+    <col min="1" max="2" width="12.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="18"/>
+    <col min="5" max="5" width="14.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3546,10 +3682,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>8</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3562,6 +3701,9 @@
       <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="27" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
@@ -3573,6 +3715,9 @@
       <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="E3" s="28" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
@@ -3582,6 +3727,9 @@
         <v>8</v>
       </c>
       <c r="C4" s="7"/>
+      <c r="E4" s="28" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
@@ -3606,10 +3754,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3660,7 +3808,7 @@
       </c>
       <c r="C12">
         <f>Backlog_AGGRAN!M5</f>
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="H12"/>
     </row>
@@ -3685,13 +3833,13 @@
       </c>
       <c r="C14">
         <f>Backlog_AGGRAN!M6</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="H14"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="18" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>11</v>
@@ -3718,12 +3866,12 @@
         <v>26</v>
       </c>
       <c r="B22" s="18">
-        <f t="shared" ref="B22:B23" si="0">SUMIFS(C10:C15,A10:A15,A22,B10:B15,B$20)</f>
+        <f>SUMIFS(C10:C15,A10:A15,A22,B10:B15,B$20)</f>
         <v>79</v>
       </c>
       <c r="C22" s="18">
         <f>SUMIFS(C9:C14,A9:A14,A22,B9:B14,C$20)</f>
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3731,12 +3879,12 @@
         <v>30</v>
       </c>
       <c r="B23" s="18">
-        <f t="shared" si="0"/>
+        <f>SUMIFS(C11:C16,A11:A16,A23,B11:B16,B$20)</f>
         <v>144</v>
       </c>
       <c r="C23" s="18">
-        <f t="shared" ref="C22:C23" si="1">SUMIFS(C11:C16,A11:A16,A23,B11:B16,C$20)</f>
-        <v>0</v>
+        <f t="shared" ref="C23" si="0">SUMIFS(C11:C16,A11:A16,A23,B11:B16,C$20)</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3751,5 +3899,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6FF80C7-5690-4C60-8231-37AF59A55C3B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6FF80C7-5690-4C60-8231-37AF59A55C3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Versão final - Backlog e Menual de Instalação
</commit_message>
<xml_diff>
--- a/Documentação/GraficoBurndown_aggran_grupo09.xlsx
+++ b/Documentação/GraficoBurndown_aggran_grupo09.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesley.souza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d47aa5dd819dd88/Desktop/Aggran-Grupo-9/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC4E9840-4199-44F7-BC07-94FB6D44FCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{CC4E9840-4199-44F7-BC07-94FB6D44FCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92BBE49C-72CE-4A53-92C8-83C5FCE7CB49}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A7B2C129-0DC2-486F-98D2-A2B5534F11BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A7B2C129-0DC2-486F-98D2-A2B5534F11BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog_AGGRAN" sheetId="5" r:id="rId1"/>
@@ -1399,7 +1399,7 @@
                   <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2578,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C44B03-923B-4AFE-8D99-0AB4AE36770F}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2818,11 +2818,11 @@
       </c>
       <c r="M6" s="2">
         <f>SUMIFS(Tabela2[TAM('#)],Tabela2[STATUS],$M$2,Tabela2[SPRINT],$J6)</f>
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="N6" s="2">
         <f>L6-M6</f>
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -3224,7 +3224,7 @@
         <v>30</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3250,7 +3250,7 @@
         <v>30</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3276,7 +3276,7 @@
         <v>30</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3302,7 +3302,7 @@
         <v>30</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -3328,7 +3328,7 @@
         <v>30</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -3380,7 +3380,7 @@
         <v>30</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -3406,7 +3406,7 @@
         <v>30</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -3484,7 +3484,7 @@
         <v>30</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -3536,7 +3536,7 @@
         <v>30</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -3562,7 +3562,7 @@
         <v>30</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -3588,7 +3588,7 @@
         <v>30</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -3614,7 +3614,7 @@
         <v>30</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="C14">
         <f>Backlog_AGGRAN!M6</f>
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="H14"/>
     </row>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C23" s="18">
         <f t="shared" ref="C23" si="0">SUMIFS(C11:C16,A11:A16,A23,B11:B16,C$20)</f>
-        <v>31</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>